<commit_message>
Energy Aspects import watcher.
</commit_message>
<xml_diff>
--- a/tests/data/test_excel_extractor.xlsx
+++ b/tests/data/test_excel_extractor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Projects\Analytics\Python37\adub\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\Analytics\adub\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4702AE4-60DF-4EF0-ABEE-23EF91003115}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0386279-BE39-4000-97BE-DBA9F6E91975}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22515" yWindow="2640" windowWidth="21600" windowHeight="9405" xr2:uid="{091385F7-75F2-4128-A47D-1B8B1E0D1EC6}"/>
+    <workbookView xWindow="672" yWindow="780" windowWidth="17280" windowHeight="9024" xr2:uid="{091385F7-75F2-4128-A47D-1B8B1E0D1EC6}"/>
   </bookViews>
   <sheets>
     <sheet name="one column one block" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>a</t>
   </si>
@@ -57,55 +57,7 @@
     <t>h</t>
   </si>
   <si>
-    <t>l</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>p</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>r</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>t</t>
-  </si>
-  <si>
-    <t>u</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>w</t>
-  </si>
-  <si>
-    <t>x</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>z</t>
-  </si>
-  <si>
     <t>test</t>
-  </si>
-  <si>
-    <t>another</t>
   </si>
 </sst>
 </file>
@@ -457,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63ED305D-F70A-49D7-BE0C-F04BD45E4EE0}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C27"/>
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
@@ -473,10 +425,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -484,10 +436,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -495,10 +447,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -506,10 +458,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -517,10 +469,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -528,10 +480,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -539,10 +491,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -550,183 +502,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>12</v>
-      </c>
-      <c r="B12" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>14</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>24</v>
-      </c>
-      <c r="B24" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>25</v>
-      </c>
-      <c r="B25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>26</v>
-      </c>
-      <c r="B26" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>27</v>
-      </c>
-      <c r="B27" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>